<commit_message>
Pulling variables for stunting analysis
</commit_message>
<xml_diff>
--- a/R/Excel/hh_vars_tokeep.xlsx
+++ b/R/Excel/hh_vars_tokeep.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="3320" windowWidth="25000" windowHeight="11560" tabRatio="500"/>
+    <workbookView xWindow="14460" yWindow="1060" windowWidth="27500" windowHeight="15240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="hh_labels.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4726" uniqueCount="2659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4728" uniqueCount="2661">
   <si>
     <t>var</t>
   </si>
@@ -7996,6 +7996,12 @@
   </si>
   <si>
     <t>wealth_index</t>
+  </si>
+  <si>
+    <t>cluster_num</t>
+  </si>
+  <si>
+    <t>num_kids</t>
   </si>
 </sst>
 </file>
@@ -8051,8 +8057,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -8066,15 +8076,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8406,8 +8420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8451,803 +8465,809 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2610</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>2617</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>2620</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>2622</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>2612</v>
+        <v>2622</v>
       </c>
       <c r="E8" t="s">
-        <v>2613</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>2615</v>
+        <v>2612</v>
       </c>
       <c r="E9" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>2611</v>
+        <v>2615</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2614</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>2616</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>2624</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>2619</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>2626</v>
+        <v>2619</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>2618</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>2586</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>2628</v>
-      </c>
-      <c r="E19" t="s">
-        <v>77</v>
+      <c r="D19" t="s">
+        <v>2586</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>2590</v>
+      <c r="D20" s="1" t="s">
+        <v>2628</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>2589</v>
+        <v>2590</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>2608</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>2602</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>2629</v>
-      </c>
-      <c r="E40" t="s">
-        <v>2636</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="E41" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="E42" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="E43" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="E44" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="E45" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="E46" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>2646</v>
+        <v>2635</v>
       </c>
       <c r="E47" t="s">
-        <v>2649</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="E48" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="E49" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>222</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s">
-        <v>223</v>
+        <v>127</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>2644</v>
+        <v>2648</v>
       </c>
       <c r="E50" t="s">
-        <v>2645</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B51" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>2652</v>
+        <v>2644</v>
       </c>
       <c r="E51" t="s">
-        <v>2655</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B52" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="E52" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B53" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="E53" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>228</v>
       </c>
       <c r="B54" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>2658</v>
+        <v>2654</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2657</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>198</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>199</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>2658</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -9314,7 +9334,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -9322,7 +9342,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>50</v>
       </c>
@@ -9330,7 +9350,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>56</v>
       </c>
@@ -9338,7 +9358,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>60</v>
       </c>
@@ -9346,7 +9366,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>62</v>
       </c>
@@ -9354,7 +9374,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -9362,15 +9382,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>66</v>
       </c>
       <c r="B71" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -9378,7 +9404,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -9386,7 +9412,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -9394,7 +9420,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -9402,7 +9428,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>106</v>
       </c>
@@ -9410,7 +9436,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>128</v>
       </c>
@@ -9418,7 +9444,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>130</v>
       </c>
@@ -9426,7 +9452,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>132</v>
       </c>
@@ -9434,7 +9460,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>134</v>
       </c>

</xml_diff>